<commit_message>
Atualiza README e Documentação
Último commit do projeto. Foi um sucesso
</commit_message>
<xml_diff>
--- a/Documentos/Cronograma_Grupo-9.xlsx
+++ b/Documentos/Cronograma_Grupo-9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos\Desktop\Final\WSTowerApp\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos\Documents\GitHub\WSTowerApp\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DF27520-0280-4B29-8B0F-3E09D0B25523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A116CD-30DE-4AB7-8DD2-3008A4532B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Atividade</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Testes Postman</t>
-  </si>
-  <si>
-    <t>Em Desenvolvimento</t>
   </si>
   <si>
     <t>Aplicação Mobile(Front-End)</t>
@@ -435,7 +432,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -516,7 +513,7 @@
         <v>44032</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="14"/>
       <c r="M5" s="9" t="s">
@@ -534,7 +531,7 @@
         <v>44033</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="14"/>
       <c r="M6" s="9" t="s">
@@ -552,7 +549,7 @@
         <v>44036</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" s="14"/>
       <c r="M7" s="4" t="s">
@@ -566,13 +563,13 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6">
         <v>44032</v>
@@ -592,7 +589,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6">
         <v>44032</v>
@@ -612,7 +609,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="6">
         <v>44034</v>
@@ -632,7 +629,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="6">
         <v>44036</v>
@@ -641,7 +638,7 @@
         <v>44036</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="4" t="s">
@@ -650,13 +647,13 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="6">
         <v>44032</v>
@@ -665,7 +662,7 @@
         <v>44033</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -675,7 +672,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="6">
         <v>44032</v>
@@ -684,7 +681,7 @@
         <v>44032</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="14"/>
       <c r="M16" s="9" t="s">
@@ -693,20 +690,22 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="6">
-        <v>44036</v>
+        <v>44034</v>
       </c>
       <c r="C17" s="7">
         <v>44036</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -714,15 +713,15 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>